<commit_message>
ignore office lock files
</commit_message>
<xml_diff>
--- a/grid_math.xlsx
+++ b/grid_math.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t xml:space="preserve">longitide</t>
+    <t xml:space="preserve">longitude</t>
   </si>
   <si>
     <t xml:space="preserve">latitude</t>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">2. divide by long by 20, lat by 10</t>
   </si>
   <si>
-    <t xml:space="preserve">3. int parts are first two grid charcters</t>
+    <t xml:space="preserve">3. int parts are first two grid characters</t>
   </si>
   <si>
     <t xml:space="preserve">A=0, B=1, etc</t>
@@ -384,8 +384,8 @@
   </sheetPr>
   <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>